<commit_message>
Creación de plantilla para subir datos a la base de datos y correción de la carga de datos
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\seguridadsocial2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48813555-5B33-4DF4-B8B8-5BDF2510B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EB87D4-C128-4B6E-ABF0-EE2191F54FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{419F8BA7-0E05-48A7-BD07-EF9600213DE2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Nombre</t>
   </si>
@@ -190,6 +190,33 @@
   </si>
   <si>
     <t>seve</t>
+  </si>
+  <si>
+    <t>Larry</t>
+  </si>
+  <si>
+    <t>Zimmerman2</t>
+  </si>
+  <si>
+    <t>Zimmerman1</t>
+  </si>
+  <si>
+    <t>malvinas2</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>garcía</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>philips</t>
   </si>
 </sst>
 </file>
@@ -557,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A4AC57E-8DDE-45B0-8E12-D0D4F17E64A2}">
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,7 +1052,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>46</v>
@@ -1081,7 +1108,7 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -1194,6 +1221,44 @@
       </c>
       <c r="C12">
         <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="5">
+        <v>31695</v>
+      </c>
+      <c r="E16" s="5">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>